<commit_message>
With parser and  filter
</commit_message>
<xml_diff>
--- a/mongo_xlsx_bridge/output/sample.xlsx
+++ b/mongo_xlsx_bridge/output/sample.xlsx
@@ -14,37 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>DB1 IDs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[{"ID#":904556601}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556602}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556603}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB2 Col1 Email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"hikmet75@vt.edu"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"smctigue@vt.edu"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"yinggeli@vt.edu"</t>
+    <t>904556602</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB1 Col2 Position Numbers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1472910</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1416345</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1458171</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -52,15 +44,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[{"ID#":904556607,"Name":"Hikmet Gursoy","Title":"Associate Director of IT","Position Number":1472910,"Department":"DSA Non IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-9573","Email":"hikmet75@vt.edu","Location":"417 Clay St","Superviser ID":904556600,"Supervisor Position Number":531599,"Reviever ID":904556600,"Reviever Position Number":531599}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556608,"Name":"Steven McTigue","Title":"Assistant Director of IT","Position Number":1416345,"Department":"DSA IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-5538","Email":"smctigue@vt.edu","Location":"417 Clay St","Superviser ID":904556601,"Supervisor Position Number":472910,"Reviever ID":904556600,"Reviever Position Number":531599}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556609,"Name":"Yingge Li","Title":"Application Developer","Position Number":1458171,"Department":"DSA IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-4612","Email":"yinggeli@vt.edu","Location":"NHW","Superviser ID":904556601,"Supervisor Position Number":472910,"Reviever ID":904556600,"Reviever Position Number":531599}]</t>
+    <t>ID#:904556607,Name:Hikmet Gursoy,Title:Associate Director of IT,Position Number:1472910,Department:DSA Non IT,Dpt Number:655523,ORG Number:40903,Number:231-9573,Email:hikmet75@vt.edu,Location:417 Clay St,Superviser ID:904556600,Supervisor Position Number:531599,Reviever ID:904556600,Reviever Position Number:531599</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#:904556608,Name:Steven McTigue,Title:Assistant Director of IT,Position Number:1416345,Department:DSA IT,Dpt Number:655523,ORG Number:40903,Number:231-5538,Email:smctigue@vt.edu,Location:417 Clay St,Superviser ID:904556601,Supervisor Position Number:472910,Reviever ID:904556600,Reviever Position Number:531599</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#:904556609,Name:Yingge Li,Title:Application Developer,Position Number:1458171,Department:DSA IT,Dpt Number:655523,ORG Number:40903,Number:231-4612,Email:yinggeli@vt.edu,Location:NHW,Superviser ID:904556601,Supervisor Position Number:472910,Reviever ID:904556600,Reviever Position Number:531599</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2 Col1 Email &amp; Username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Steven McTigue,smctigue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yingge Li,yinggeli</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2 Col2 Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hikmet75@vt.edu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB2 Col3 Email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hikmet75@vt.edu,Hikmet Gursoy,1472910</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -68,35 +88,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"csteph@vt.edu"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"aaron86@vt.edu "</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"bmike@vt.edu"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB1 Col2 Position Numbers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"Position Number":1472910}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"Position Number":1416345}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"Position Number":1458171}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB2 Col2 Email</t>
+    <t>csteph@vt.edu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaron86@vt.edu </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bmike@vt.edu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB3 Col2 Attributes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#:904556634,Name:Stephen Chamberlin,Title:Computer Support Specialist,Position Number:444346,Department:DSA IT,Dpt Number:655523,ORG Number:40903,Number:231-2303,Email:csteph@vt.edu,Location:Squires Student Center,Superviser ID:904556606,Supervisor Position Number:533101,Reviever ID:904556602,Reviever Position Number:416345</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#:904556635,Name:Aaron Weekly,Title:Computer Support Specialist,Position Number:531599,Department:DSA IT,Dpt Number:655523,ORG Number:40903,Number:231-2303,Email:aaron86@vt.edu ,Location:Squires Student Center,Superviser ID:904556606,Supervisor Position Number:533101,Reviever ID:904556602,Reviever Position Number:416345</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID#:904556636,Name:Mike Burns,Title:Computer Support Specialist,Position Number:466131,Department:DSA IT,Dpt Number:655523,ORG Number:40903,Number:231-7509,Email:bmike@vt.edu,Location:NHW,Superviser ID:904556606,Supervisor Position Number:533101,Reviever ID:904556602,Reviever Position Number:416345</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -104,35 +120,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"csteph"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"aaron86"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"bmike"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB3 Col2 Attributes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556634,"Name":"Stephen Chamberlin","Title":"Computer Support Specialist","Position Number":444346,"Department":"DSA IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-2303","Email":"csteph@vt.edu","Location":"Squires Student Center","Superviser ID":904556606,"Supervisor Position Number":533101,"Reviever ID":904556602,"Reviever Position Number":416345}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556635,"Name":"Aaron Weekly","Title":"Computer Support Specialist","Position Number":531599,"Department":"DSA IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-2303","Email":"aaron86@vt.edu ","Location":"Squires Student Center","Superviser ID":904556606,"Supervisor Position Number":533101,"Reviever ID":904556602,"Reviever Position Number":416345}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[{"ID#":904556636,"Name":"Mike Burns","Title":"Computer Support Specialist","Position Number":466131,"Department":"DSA IT","Dpt Number":655523,"ORG Number":40903,"Number":"231-7509","Email":"bmike@vt.edu","Location":"NHW","Superviser ID":904556606,"Supervisor Position Number":533101,"Reviever ID":904556602,"Reviever Position Number":416345}]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB2 Col3 Email</t>
+    <t>csteph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaron86</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bmike</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -470,218 +466,197 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:100">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:100">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:100">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:100">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:100"/>
-    <row r="6" spans="1:100"/>
-    <row r="7" spans="1:100"/>
-    <row r="8" spans="1:100"/>
-    <row r="9" spans="1:100"/>
-    <row r="10" spans="1:100"/>
-    <row r="11" spans="1:100"/>
-    <row r="12" spans="1:100"/>
-    <row r="13" spans="1:100"/>
-    <row r="14" spans="1:100"/>
-    <row r="15" spans="1:100"/>
-    <row r="16" spans="1:100"/>
-    <row r="17" spans="1:100"/>
-    <row r="18" spans="1:100"/>
-    <row r="19" spans="1:100"/>
-    <row r="20" spans="1:100"/>
-    <row r="21" spans="1:100"/>
-    <row r="22" spans="1:100"/>
-    <row r="23" spans="1:100"/>
-    <row r="24" spans="1:100"/>
-    <row r="25" spans="1:100"/>
-    <row r="26" spans="1:100"/>
-    <row r="27" spans="1:100"/>
-    <row r="28" spans="1:100"/>
-    <row r="29" spans="1:100"/>
-    <row r="30" spans="1:100"/>
-    <row r="31" spans="1:100"/>
-    <row r="32" spans="1:100"/>
-    <row r="33" spans="1:100"/>
-    <row r="34" spans="1:100"/>
-    <row r="35" spans="1:100"/>
-    <row r="36" spans="1:100"/>
-    <row r="37" spans="1:100"/>
-    <row r="38" spans="1:100"/>
-    <row r="39" spans="1:100"/>
-    <row r="40" spans="1:100"/>
-    <row r="41" spans="1:100"/>
-    <row r="42" spans="1:100"/>
-    <row r="43" spans="1:100"/>
-    <row r="44" spans="1:100"/>
-    <row r="45" spans="1:100"/>
-    <row r="46" spans="1:100"/>
-    <row r="47" spans="1:100"/>
-    <row r="48" spans="1:100"/>
-    <row r="49" spans="1:100"/>
-    <row r="50" spans="1:100"/>
-    <row r="51" spans="1:100"/>
-    <row r="52" spans="1:100"/>
-    <row r="53" spans="1:100"/>
-    <row r="54" spans="1:100"/>
-    <row r="55" spans="1:100"/>
-    <row r="56" spans="1:100"/>
-    <row r="57" spans="1:100"/>
-    <row r="58" spans="1:100"/>
-    <row r="59" spans="1:100"/>
-    <row r="60" spans="1:100"/>
-    <row r="61" spans="1:100"/>
-    <row r="62" spans="1:100"/>
-    <row r="63" spans="1:100"/>
-    <row r="64" spans="1:100"/>
-    <row r="65" spans="1:100"/>
-    <row r="66" spans="1:100"/>
-    <row r="67" spans="1:100"/>
-    <row r="68" spans="1:100"/>
-    <row r="69" spans="1:100"/>
-    <row r="70" spans="1:100"/>
-    <row r="71" spans="1:100"/>
-    <row r="72" spans="1:100"/>
-    <row r="73" spans="1:100"/>
-    <row r="74" spans="1:100"/>
-    <row r="75" spans="1:100"/>
-    <row r="76" spans="1:100"/>
-    <row r="77" spans="1:100"/>
-    <row r="78" spans="1:100"/>
-    <row r="79" spans="1:100"/>
-    <row r="80" spans="1:100"/>
-    <row r="81" spans="1:100"/>
-    <row r="82" spans="1:100"/>
-    <row r="83" spans="1:100"/>
-    <row r="84" spans="1:100"/>
-    <row r="85" spans="1:100"/>
-    <row r="86" spans="1:100"/>
-    <row r="87" spans="1:100"/>
-    <row r="88" spans="1:100"/>
-    <row r="89" spans="1:100"/>
-    <row r="90" spans="1:100"/>
-    <row r="91" spans="1:100"/>
-    <row r="92" spans="1:100"/>
-    <row r="93" spans="1:100"/>
-    <row r="94" spans="1:100"/>
-    <row r="95" spans="1:100"/>
-    <row r="96" spans="1:100"/>
-    <row r="97" spans="1:100"/>
-    <row r="98" spans="1:100"/>
-    <row r="99" spans="1:100"/>
-    <row r="100" spans="1:100"/>
+    <row r="5" spans="1:9"/>
+    <row r="6" spans="1:9"/>
+    <row r="7" spans="1:9"/>
+    <row r="8" spans="1:9"/>
+    <row r="9" spans="1:9"/>
+    <row r="10" spans="1:9"/>
+    <row r="11" spans="1:9"/>
+    <row r="12" spans="1:9"/>
+    <row r="13" spans="1:9"/>
+    <row r="14" spans="1:9"/>
+    <row r="15" spans="1:9"/>
+    <row r="16" spans="1:9"/>
+    <row r="17" spans="1:9"/>
+    <row r="18" spans="1:9"/>
+    <row r="19" spans="1:9"/>
+    <row r="20" spans="1:9"/>
+    <row r="21" spans="1:9"/>
+    <row r="22" spans="1:9"/>
+    <row r="23" spans="1:9"/>
+    <row r="24" spans="1:9"/>
+    <row r="25" spans="1:9"/>
+    <row r="26" spans="1:9"/>
+    <row r="27" spans="1:9"/>
+    <row r="28" spans="1:9"/>
+    <row r="29" spans="1:9"/>
+    <row r="30" spans="1:9"/>
+    <row r="31" spans="1:9"/>
+    <row r="32" spans="1:9"/>
+    <row r="33" spans="1:9"/>
+    <row r="34" spans="1:9"/>
+    <row r="35" spans="1:9"/>
+    <row r="36" spans="1:9"/>
+    <row r="37" spans="1:9"/>
+    <row r="38" spans="1:9"/>
+    <row r="39" spans="1:9"/>
+    <row r="40" spans="1:9"/>
+    <row r="41" spans="1:9"/>
+    <row r="42" spans="1:9"/>
+    <row r="43" spans="1:9"/>
+    <row r="44" spans="1:9"/>
+    <row r="45" spans="1:9"/>
+    <row r="46" spans="1:9"/>
+    <row r="47" spans="1:9"/>
+    <row r="48" spans="1:9"/>
+    <row r="49" spans="1:9"/>
+    <row r="50" spans="1:9"/>
+    <row r="51" spans="1:9"/>
+    <row r="52" spans="1:9"/>
+    <row r="53" spans="1:9"/>
+    <row r="54" spans="1:9"/>
+    <row r="55" spans="1:9"/>
+    <row r="56" spans="1:9"/>
+    <row r="57" spans="1:9"/>
+    <row r="58" spans="1:9"/>
+    <row r="59" spans="1:9"/>
+    <row r="60" spans="1:9"/>
+    <row r="61" spans="1:9"/>
+    <row r="62" spans="1:9"/>
+    <row r="63" spans="1:9"/>
+    <row r="64" spans="1:9"/>
+    <row r="65" spans="1:9"/>
+    <row r="66" spans="1:9"/>
+    <row r="67" spans="1:9"/>
+    <row r="68" spans="1:9"/>
+    <row r="69" spans="1:9"/>
+    <row r="70" spans="1:9"/>
+    <row r="71" spans="1:9"/>
+    <row r="72" spans="1:9"/>
+    <row r="73" spans="1:9"/>
+    <row r="74" spans="1:9"/>
+    <row r="75" spans="1:9"/>
+    <row r="76" spans="1:9"/>
+    <row r="77" spans="1:9"/>
+    <row r="78" spans="1:9"/>
+    <row r="79" spans="1:9"/>
+    <row r="80" spans="1:9"/>
+    <row r="81" spans="1:9"/>
+    <row r="82" spans="1:9"/>
+    <row r="83" spans="1:9"/>
+    <row r="84" spans="1:9"/>
+    <row r="85" spans="1:9"/>
+    <row r="86" spans="1:9"/>
+    <row r="87" spans="1:9"/>
+    <row r="88" spans="1:9"/>
+    <row r="89" spans="1:9"/>
+    <row r="90" spans="1:9"/>
+    <row r="91" spans="1:9"/>
+    <row r="92" spans="1:9"/>
+    <row r="93" spans="1:9"/>
+    <row r="94" spans="1:9"/>
+    <row r="95" spans="1:9"/>
+    <row r="96" spans="1:9"/>
+    <row r="97" spans="1:9"/>
+    <row r="98" spans="1:9"/>
+    <row r="99" spans="1:9"/>
+    <row r="100" spans="1:9"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>